<commit_message>
Adding 1/5 patches of phase 1 plot.
- Added entry forvertical subside hook 27
- want to patch first then plot layer for visibility in future dev.
</commit_message>
<xml_diff>
--- a/Datas/patchtables.xlsx
+++ b/Datas/patchtables.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Istamosh\Desktop\ODE\GBB\Project\Project Siteplan Plot\SiteplanColorPlot\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ODE\Workspace\GitHub Projects\SiteplanColorPlot\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83C4F95-E555-4B42-A47C-EDFDE672298A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A985EF64-7C2F-4272-AD0D-4D341F6E1612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="10245" windowHeight="10920" xr2:uid="{199A0DCC-37CE-46E7-9F90-BF58DEF6FA53}"/>
+    <workbookView xWindow="1380" yWindow="3405" windowWidth="10245" windowHeight="6000" xr2:uid="{199A0DCC-37CE-46E7-9F90-BF58DEF6FA53}"/>
   </bookViews>
   <sheets>
     <sheet name="patchtables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>code</t>
   </si>
@@ -97,6 +103,9 @@
   </si>
   <si>
     <t>chartreuse</t>
+  </si>
+  <si>
+    <t>springgreen</t>
   </si>
 </sst>
 </file>
@@ -182,10 +191,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63309D44-1FF3-4200-A984-A44F486645E7}" name="Table1" displayName="Table1" ref="A1:I10" totalsRowShown="0">
-  <autoFilter ref="A1:I10" xr:uid="{63309D44-1FF3-4200-A984-A44F486645E7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I10">
-    <sortCondition ref="D1:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63309D44-1FF3-4200-A984-A44F486645E7}" name="Table1" displayName="Table1" ref="A1:I14" totalsRowShown="0">
+  <autoFilter ref="A1:I14" xr:uid="{63309D44-1FF3-4200-A984-A44F486645E7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I13">
+    <sortCondition ref="D1:D13"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{1075CE5D-477F-4D2A-939D-C15D79C3424F}" name="code" dataDxfId="7">
@@ -198,13 +207,13 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DFD14808-7748-40DC-B47C-AD3993DCC6F0}" name="orient"/>
     <tableColumn id="7" xr3:uid="{06623992-763C-499D-8C0F-1E2DAE6B1D7D}" name="extra" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E75AC792-2743-4751-B83D-BC51B636560A}" name="expandx" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{E75AC792-2743-4751-B83D-BC51B636560A}" name="expandx" dataDxfId="2">
       <calculatedColumnFormula>IF(E2="v", VLOOKUP(B2, $K$2:$M$4,2)+F2, VLOOKUP(B2,$K$2:$M$4,3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D709E13A-9272-44EA-88E3-5C7F3CDDADA9}" name="expandy" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{D709E13A-9272-44EA-88E3-5C7F3CDDADA9}" name="expandy" dataDxfId="1">
       <calculatedColumnFormula>IF(E2="v", VLOOKUP(B2,$K$2:$M$4, 3), VLOOKUP(B2,$K$2:$M$4,2)+F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2AEC1907-52E1-4AAD-BA01-64D29D0AFE76}" name="color" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2AEC1907-52E1-4AAD-BA01-64D29D0AFE76}" name="color" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -507,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D8DAFC-B19E-44AE-A92D-62DE394D1006}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,34 +608,30 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E3&amp;C3</f>
-        <v>subv25</v>
+        <v>subh</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2">
-        <v>25</v>
-      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="str">
         <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>27/60 (6x10) +25</v>
+        <v>27/60 (6x10)</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1">
-        <v>30</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1">
         <f>IF(E3="v", VLOOKUP(B3, $K$2:$M$4,2)+F3, VLOOKUP(B3,$K$2:$M$4,3))</f>
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="H3" s="1">
         <f>IF(E3="v", VLOOKUP(B3,$K$2:$M$4, 3), VLOOKUP(B3,$K$2:$M$4,2)+F3)</f>
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" t="s">
@@ -640,36 +645,36 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+      <c r="A4" s="2" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E4&amp;C4</f>
-        <v>subv30</v>
-      </c>
-      <c r="B4" t="s">
+        <v>subv25</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>27/60 (6x10) +30</v>
+        <v>27/60 (6x10) +25</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1">
         <f>IF(E4="v", VLOOKUP(B4, $K$2:$M$4,2)+F4, VLOOKUP(B4,$K$2:$M$4,3))</f>
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H4" s="1">
         <f>IF(E4="v", VLOOKUP(B4,$K$2:$M$4, 3), VLOOKUP(B4,$K$2:$M$4,2)+F4)</f>
         <v>120</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" t="s">
@@ -685,192 +690,324 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E5&amp;C5</f>
-        <v>subv40</v>
+        <v>subv30</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>27/60 (6x10) +40</v>
+      <c r="C5" s="2">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>27/60 (6x10) +30</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1">
         <f>IF(E5="v", VLOOKUP(B5, $K$2:$M$4,2)+F5, VLOOKUP(B5,$K$2:$M$4,3))</f>
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="H5" s="1">
         <f>IF(E5="v", VLOOKUP(B5,$K$2:$M$4, 3), VLOOKUP(B5,$K$2:$M$4,2)+F5)</f>
         <v>120</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+      <c r="A6" s="2" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E6&amp;C6</f>
-        <v>comv</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>36/72 (6x12)</v>
+        <v>subh30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>27/60 (6x10) +30</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F6" s="1">
+        <v>36</v>
+      </c>
       <c r="G6" s="1">
         <f>IF(E6="v", VLOOKUP(B6, $K$2:$M$4,2)+F6, VLOOKUP(B6,$K$2:$M$4,3))</f>
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1">
         <f>IF(E6="v", VLOOKUP(B6,$K$2:$M$4, 3), VLOOKUP(B6,$K$2:$M$4,2)+F6)</f>
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="str">
+      <c r="A7" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E7&amp;C7</f>
-        <v>comh</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="str">
-        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>36/72 (6x12)</v>
+        <v>subv40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>27/60 (6x10) +40</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>48</v>
+      </c>
       <c r="G7" s="1">
         <f>IF(E7="v", VLOOKUP(B7, $K$2:$M$4,2)+F7, VLOOKUP(B7,$K$2:$M$4,3))</f>
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="H7" s="1">
         <f>IF(E7="v", VLOOKUP(B7,$K$2:$M$4, 3), VLOOKUP(B7,$K$2:$M$4,2)+F7)</f>
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="str">
+      <c r="A8" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E8&amp;C8</f>
-        <v>comh30</v>
-      </c>
-      <c r="B8" s="2" t="s">
+        <v>comv</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>36/72 (6x12) +30</v>
+      <c r="D8" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>36/72 (6x12)</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1">
         <f>IF(E8="v", VLOOKUP(B8, $K$2:$M$4,2)+F8, VLOOKUP(B8,$K$2:$M$4,3))</f>
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="H8" s="1">
         <f>IF(E8="v", VLOOKUP(B8,$K$2:$M$4, 3), VLOOKUP(B8,$K$2:$M$4,2)+F8)</f>
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E9&amp;C9</f>
-        <v>comv30</v>
+        <v>comh</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2">
-        <v>30</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="str">
         <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>36/72 (6x12) +30</v>
+        <v>36/72 (6x12)</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1">
-        <v>30</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1">
         <f>IF(E9="v", VLOOKUP(B9, $K$2:$M$4,2)+F9, VLOOKUP(B9,$K$2:$M$4,3))</f>
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="H9" s="1">
         <f>IF(E9="v", VLOOKUP(B9,$K$2:$M$4, 3), VLOOKUP(B9,$K$2:$M$4,2)+F9)</f>
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
+      <c r="A10" s="2" t="str">
         <f>Table1[[#This Row],[spec]]&amp;E10&amp;C10</f>
-        <v>comv36</v>
-      </c>
-      <c r="B10" t="s">
+        <v>comh30</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
-        <v>36</v>
-      </c>
-      <c r="D10" t="str">
-        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
-        <v>36/72 (6x12) +36</v>
+      <c r="C10" s="2">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>36/72 (6x12) +30</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1">
         <v>36</v>
       </c>
       <c r="G10" s="1">
         <f>IF(E10="v", VLOOKUP(B10, $K$2:$M$4,2)+F10, VLOOKUP(B10,$K$2:$M$4,3))</f>
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="H10" s="1">
         <f>IF(E10="v", VLOOKUP(B10,$K$2:$M$4, 3), VLOOKUP(B10,$K$2:$M$4,2)+F10)</f>
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="str">
+        <f>Table1[[#This Row],[spec]]&amp;E11&amp;C11</f>
+        <v>comv30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>36/72 (6x12) +30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1">
+        <f>IF(E11="v", VLOOKUP(B11, $K$2:$M$4,2)+F11, VLOOKUP(B11,$K$2:$M$4,3))</f>
+        <v>102</v>
+      </c>
+      <c r="H11" s="1">
+        <f>IF(E11="v", VLOOKUP(B11,$K$2:$M$4, 3), VLOOKUP(B11,$K$2:$M$4,2)+F11)</f>
+        <v>144</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>Table1[[#This Row],[spec]]&amp;E12&amp;C12</f>
+        <v>comv36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>36</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>36/72 (6x12) +36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(E12="v", VLOOKUP(B12, $K$2:$M$4,2)+F12, VLOOKUP(B12,$K$2:$M$4,3))</f>
+        <v>108</v>
+      </c>
+      <c r="H12" s="1">
+        <f>IF(E12="v", VLOOKUP(B12,$K$2:$M$4, 3), VLOOKUP(B12,$K$2:$M$4,2)+F12)</f>
+        <v>144</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="str">
+        <f>Table1[[#This Row],[spec]]&amp;E13&amp;C13</f>
+        <v>comh36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>36/72 (6x12) +36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1">
+        <v>36</v>
+      </c>
+      <c r="G13" s="1">
+        <f>IF(E13="v", VLOOKUP(B13, $K$2:$M$4,2)+F13, VLOOKUP(B13,$K$2:$M$4,3))</f>
+        <v>144</v>
+      </c>
+      <c r="H13" s="1">
+        <f>IF(E13="v", VLOOKUP(B13,$K$2:$M$4, 3), VLOOKUP(B13,$K$2:$M$4,2)+F13)</f>
+        <v>108</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="str">
+        <f>Table1[[#This Row],[spec]]&amp;E14&amp;C14</f>
+        <v>subv27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>IF(Table1[[#This Row],[spec]]="com","36/72 (6x12)",IF(Table1[[#This Row],[spec]]="sub","27/60 (6x10)","27/60 (5x12)"))&amp;IF(Table1[[#This Row],[hooktype]]="",""," +"&amp;Table1[[#This Row],[hooktype]])</f>
+        <v>27/60 (6x10) +27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>36</v>
+      </c>
+      <c r="G14" s="1">
+        <f>IF(E14="v", VLOOKUP(B14, $K$2:$M$4,2)+F14, VLOOKUP(B14,$K$2:$M$4,3))</f>
+        <v>108</v>
+      </c>
+      <c r="H14" s="1">
+        <f>IF(E14="v", VLOOKUP(B14,$K$2:$M$4, 3), VLOOKUP(B14,$K$2:$M$4,2)+F14)</f>
+        <v>120</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>